<commit_message>
Power supply almost done
</commit_message>
<xml_diff>
--- a/BOM SIUE.xlsx
+++ b/BOM SIUE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\Studia\LM331m1(1)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{295D0481-B2E2-48D4-AAC2-C58BA4B2350C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73A58315-994E-43BF-A90C-C9A5DC2CD04A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{A90BA58C-8162-4AA7-B15C-980DEFEC99B1}"/>
   </bookViews>
@@ -624,8 +624,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6506BA97-DD70-4DDD-AFD6-521D618244B3}">
   <dimension ref="A1:L20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="62" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -984,7 +984,7 @@
       <c r="C12" t="s">
         <v>35</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="2" t="s">
         <v>36</v>
       </c>
       <c r="E12">
@@ -1014,7 +1014,7 @@
       <c r="C13" t="s">
         <v>38</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="2" t="s">
         <v>39</v>
       </c>
       <c r="E13">
@@ -1258,6 +1258,8 @@
     <hyperlink ref="D8" r:id="rId10" xr:uid="{4DE42AC7-6000-4662-AD2A-7D9D0D37A2F0}"/>
     <hyperlink ref="D9" r:id="rId11" xr:uid="{4CE3E4B5-8950-4D26-9A22-00D20A9B6612}"/>
     <hyperlink ref="D11" r:id="rId12" xr:uid="{086E9803-DBFD-469A-9F14-56B3129BD55B}"/>
+    <hyperlink ref="D12" r:id="rId13" xr:uid="{D96BEC54-C981-4955-BA78-8A91C2917791}"/>
+    <hyperlink ref="D13" r:id="rId14" xr:uid="{F8602EF4-B695-4EE4-B5CD-BECD4E0E2E13}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>